<commit_message>
Need protocol for final push
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/cdaniels/uofc_data/ubs_seq/Projects/tmp_lambda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/cdaniels/uofc_data/ubs_seq/Projects/UBS-seq_241002/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF339D7-6D17-104B-9854-0E63549C449A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA0EF50-FD38-9947-B9C2-AB4B3FE4EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1740" windowWidth="29140" windowHeight="19860" xr2:uid="{ED8E8DCD-5B4B-C946-9AC4-CCA3E7DD03A7}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
-    <t>Content</t>
-  </si>
-  <si>
     <t>qPCR</t>
   </si>
   <si>
@@ -59,355 +56,40 @@
     <t>ATCACG</t>
   </si>
   <si>
-    <t>A-1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 55C 60 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method A</t>
-    </r>
-  </si>
-  <si>
     <t>CGATGT</t>
   </si>
   <si>
-    <t>A-2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 50C 90 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method A</t>
-    </r>
-  </si>
-  <si>
     <t>TGACCA</t>
   </si>
   <si>
-    <t>A-3</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 50C 120 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method A</t>
-    </r>
-  </si>
-  <si>
     <t>ACAGTG</t>
   </si>
   <si>
-    <t>A-4</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 45C 4 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method A</t>
-    </r>
-  </si>
-  <si>
     <t>GCCAAT</t>
   </si>
   <si>
-    <t>B-1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 55C 60 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>CAGATC</t>
   </si>
   <si>
-    <t>B-2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 50C 90 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>ACTTGA</t>
   </si>
   <si>
-    <t>B-3</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 50C 120 mins, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>GATCAG</t>
   </si>
   <si>
-    <t>B-4</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 45C 4 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>TAGCTT</t>
   </si>
   <si>
-    <t>B-7</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 37C 8 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>GGCTAC</t>
   </si>
   <si>
-    <t>B-8</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 40C 16 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>CTTGTA</t>
   </si>
   <si>
-    <t>B-9</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 37C 16 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>AGTCAA</t>
   </si>
   <si>
-    <t>B-10</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 ng ligated DNA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BS + DNA protect buffer, 30C 16 hrs, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>method B</t>
-    </r>
-  </si>
-  <si>
     <t>AGTTCC</t>
-  </si>
-  <si>
-    <t>B-11</t>
   </si>
   <si>
     <r>
@@ -448,46 +130,124 @@
     <t>Control</t>
   </si>
   <si>
-    <t>55C 60 mins, method A</t>
-  </si>
-  <si>
-    <t>50C 90 mins, method A</t>
-  </si>
-  <si>
-    <t>50C 120 mins, method A</t>
-  </si>
-  <si>
-    <t>45C 4 hrs, method A</t>
-  </si>
-  <si>
-    <t>55C 60 mins, method B</t>
-  </si>
-  <si>
-    <t>50C 90 mins, method B</t>
-  </si>
-  <si>
-    <t>50C 120 mins, method B</t>
-  </si>
-  <si>
-    <t>45C 4 hrs, method B</t>
-  </si>
-  <si>
-    <t>37C 8 hrs, method B</t>
-  </si>
-  <si>
-    <t>40C 16 hrs, method B</t>
-  </si>
-  <si>
-    <t>37C 16 hrs, method B</t>
-  </si>
-  <si>
-    <t>30C 16 hrs, method B</t>
-  </si>
-  <si>
-    <t>25C 16 hrs, method B</t>
-  </si>
-  <si>
     <t>Recipe</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 55C 60 mins, A</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 50C 90 mins, A</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 50C 120 mins, A</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 45C 4 hrs, A</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 55C 60 mins, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 50C 90 mins, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 50C 120 mins, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 45C 4 hrs, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 37C 8 hrs, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 40C 16 hrs, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 37C 16 hrs, B</t>
+  </si>
+  <si>
+    <t>2 ng ligated DNA, BS + DNA protect buffer, 30C 16 hrs, B</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>55C 60m A</t>
+  </si>
+  <si>
+    <t>50C 90m A</t>
+  </si>
+  <si>
+    <t>50C 120m A</t>
+  </si>
+  <si>
+    <t>45C 4h A</t>
+  </si>
+  <si>
+    <t>55C 60m B</t>
+  </si>
+  <si>
+    <t>50C 90m B</t>
+  </si>
+  <si>
+    <t>50C 120m B</t>
+  </si>
+  <si>
+    <t>45C 4h B</t>
+  </si>
+  <si>
+    <t>37C 8h B</t>
+  </si>
+  <si>
+    <t>40C 16h B</t>
+  </si>
+  <si>
+    <t>37C 16h B</t>
+  </si>
+  <si>
+    <t>30C 16h B</t>
+  </si>
+  <si>
+    <t>25C 16h B</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +765,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,36 +776,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6">
         <v>10.4</v>
@@ -1057,21 +817,21 @@
         <v>1.43</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11">
         <v>12.1</v>
@@ -1083,21 +843,21 @@
         <v>1.91</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G3" s="12">
         <v>2</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="11">
         <v>15.1</v>
@@ -1109,21 +869,21 @@
         <v>2.12</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G4" s="12">
         <v>4</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="11">
         <v>8.6</v>
@@ -1135,21 +895,21 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G5" s="12">
         <v>5</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="11">
         <v>12</v>
@@ -1161,21 +921,21 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G6" s="12">
         <v>6</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7" s="15">
         <v>15.3</v>
@@ -1187,21 +947,21 @@
         <v>3.41</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G7" s="16">
         <v>7</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="15">
         <v>9</v>
@@ -1213,21 +973,21 @@
         <v>2.73</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G8" s="16">
         <v>8</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="15">
         <v>12.2</v>
@@ -1239,21 +999,21 @@
         <v>3.83</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G9" s="16">
         <v>9</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="15">
         <v>15.6</v>
@@ -1265,21 +1025,21 @@
         <v>1.83</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G10" s="16">
         <v>10</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="15">
         <v>9.6999999999999993</v>
@@ -1291,21 +1051,21 @@
         <v>2.09</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G11" s="16">
         <v>11</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" s="15">
         <v>12</v>
@@ -1317,21 +1077,21 @@
         <v>1.47</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="G12" s="16">
         <v>12</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="15">
         <v>17</v>
@@ -1343,21 +1103,21 @@
         <v>2.87</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="G13" s="16">
         <v>13</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="15">
         <v>8.6999999999999993</v>
@@ -1369,21 +1129,21 @@
         <v>2.57</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G14" s="16">
         <v>14</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="15">
         <v>15.6</v>
@@ -1395,13 +1155,13 @@
         <v>1.99</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="G15" s="16">
         <v>15</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>